<commit_message>
*changed misleading variable naming in reforms based on Hohmeyer & Wolff (2010) * removed assumed control income
</commit_message>
<xml_diff>
--- a/estimates/jobCreationSchemes.xlsx
+++ b/estimates/jobCreationSchemes.xlsx
@@ -63,42 +63,6 @@
     <t>https://ideas.repec.org/p/iab/iabdpa/201021.html</t>
   </si>
   <si>
-    <t>monthly_gross_earnings_effect_female_east_year1</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_west_year1</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_west_year1</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_east_year1</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_west_year2</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_east_year2</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_west_year2</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_east_year2</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_west_year3</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_female_east_year3</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_west_year3</t>
-  </si>
-  <si>
-    <t>monthly_gross_earnings_effect_male_east_year3</t>
-  </si>
-  <si>
     <t>Hohmeyer &amp; Wolff (2010), Table 13</t>
   </si>
   <si>
@@ -139,6 +103,42 @@
   </si>
   <si>
     <t>monthly_benefit_receipt_effect_female_west_year3</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_west_year1</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_east_year1</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_west_year1</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_east_year1</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_west_year2</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_east_year2</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_west_year2</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_east_year2</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_west_year3</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_female_east_year3</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_west_year3</t>
+  </si>
+  <si>
+    <t>yearly_gross_earnings_effect_male_east_year3</t>
   </si>
 </sst>
 </file>
@@ -963,7 +963,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3">
         <v>4157</v>
@@ -1041,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>13</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3">
         <v>4724</v>
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>13</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3">
         <v>4310</v>
@@ -1087,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>13</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3">
         <v>4324</v>
@@ -1110,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>13</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3">
         <v>2516</v>
@@ -1133,7 +1133,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>13</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B7" s="3">
         <v>1298</v>
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>13</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3">
         <v>1763</v>
@@ -1179,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>13</v>
@@ -1187,7 +1187,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B9" s="3">
         <v>804</v>
@@ -1202,7 +1202,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>13</v>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3">
         <v>1663</v>
@@ -1225,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>13</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3">
         <v>646</v>
@@ -1248,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>13</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3">
         <v>835</v>
@@ -1271,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>13</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3">
         <v>156</v>
@@ -1294,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>13</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>-236</v>
@@ -1317,7 +1317,7 @@
         <v>-1</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>13</v>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>-239</v>
@@ -1340,7 +1340,7 @@
         <v>-1</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>13</v>
@@ -1348,7 +1348,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>-267</v>
@@ -1363,7 +1363,7 @@
         <v>-1</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>13</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>-261</v>
@@ -1386,7 +1386,7 @@
         <v>-1</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>13</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1409,7 +1409,7 @@
         <v>-1</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>13</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>-23</v>
@@ -1432,7 +1432,7 @@
         <v>-1</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>13</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>-27</v>
@@ -1455,7 +1455,7 @@
         <v>-1</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>13</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>-47</v>
@@ -1478,7 +1478,7 @@
         <v>-1</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>13</v>
@@ -1486,7 +1486,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1501,7 +1501,7 @@
         <v>-1</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>13</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>-21</v>
@@ -1524,7 +1524,7 @@
         <v>-1</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>13</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>-19</v>
@@ -1547,7 +1547,7 @@
         <v>-1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>13</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>-38</v>
@@ -1570,7 +1570,7 @@
         <v>-1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>13</v>

</xml_diff>